<commit_message>
Nueva actualizacion revisen sus datos en el documento de requerimientos
Coloque nuestros nombre y en que area va a estar cada uno y hize dos nuevas historias en los criterios de aceptacion
</commit_message>
<xml_diff>
--- a/Fase 1/docRequerimientos.xlsx
+++ b/Fase 1/docRequerimientos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752"/>
   </bookViews>
   <sheets>
     <sheet name="Producto" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="61">
   <si>
     <t>Historia</t>
   </si>
@@ -89,12 +89,6 @@
     <t>Technical Director, Project Manager, Lead Engineer</t>
   </si>
   <si>
-    <t>Software Engineer</t>
-  </si>
-  <si>
-    <t>Web UI Engineer</t>
-  </si>
-  <si>
     <t>UH#-1</t>
   </si>
   <si>
@@ -186,6 +180,36 @@
   </si>
   <si>
     <t>La aplicación debe adaptarse al tamaño del dispositivo del usuario (responsive) y al idioma del mismo</t>
+  </si>
+  <si>
+    <t>Danny Caldeira</t>
+  </si>
+  <si>
+    <t>dannyelportu2013@gmail.com</t>
+  </si>
+  <si>
+    <t>BackEnd Developer</t>
+  </si>
+  <si>
+    <t>Christian Angulo</t>
+  </si>
+  <si>
+    <t>FrontEnd Developer/QA Engineer</t>
+  </si>
+  <si>
+    <t>angulo.christian@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alberto Gil Dávila </t>
+  </si>
+  <si>
+    <t>agildav@gmail.com</t>
+  </si>
+  <si>
+    <t>Maria Castro</t>
+  </si>
+  <si>
+    <t>marivicastro_94@hotmail.com</t>
   </si>
 </sst>
 </file>
@@ -298,7 +322,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -396,17 +420,6 @@
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -446,7 +459,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -476,16 +489,13 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -517,9 +527,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -531,9 +541,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Hipervínculo" xfId="2" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="4" builtinId="8"/>
-    <cellStyle name="Hipervínculo visitado" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -556,7 +566,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -842,69 +852,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E14"/>
+  <dimension ref="B2:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:E6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21.42578125" style="15" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" customWidth="1"/>
-    <col min="4" max="4" width="33.7109375" customWidth="1"/>
-    <col min="5" max="5" width="51.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.44140625" style="14" customWidth="1"/>
+    <col min="3" max="3" width="21.5546875" customWidth="1"/>
+    <col min="4" max="4" width="33.6640625" customWidth="1"/>
+    <col min="5" max="5" width="51.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="37.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:5" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" s="23"/>
-      <c r="E2" s="24"/>
-    </row>
-    <row r="3" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C2" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="22"/>
+      <c r="E2" s="23"/>
+    </row>
+    <row r="3" spans="2:5" ht="18" x14ac:dyDescent="0.3">
       <c r="B3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="26"/>
-    </row>
-    <row r="4" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D3" s="24"/>
+      <c r="E3" s="25"/>
+    </row>
+    <row r="4" spans="2:5" ht="18" x14ac:dyDescent="0.3">
       <c r="B4" s="11"/>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="27"/>
-      <c r="E4" s="28"/>
-    </row>
-    <row r="5" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D4" s="26"/>
+      <c r="E4" s="27"/>
+    </row>
+    <row r="5" spans="2:5" ht="18" x14ac:dyDescent="0.3">
       <c r="B5" s="11"/>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="27"/>
-      <c r="E5" s="28"/>
-    </row>
-    <row r="6" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D5" s="26"/>
+      <c r="E5" s="27"/>
+    </row>
+    <row r="6" spans="2:5" ht="18" x14ac:dyDescent="0.3">
       <c r="B6" s="11"/>
-      <c r="C6" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="D6" s="29"/>
-      <c r="E6" s="30"/>
-    </row>
-    <row r="7" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C6" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="28"/>
+      <c r="E6" s="29"/>
+    </row>
+    <row r="7" spans="2:5" ht="18" x14ac:dyDescent="0.3">
       <c r="B7" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="15" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="7" t="s">
@@ -914,68 +924,76 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" s="13"/>
       <c r="C8" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" s="13"/>
       <c r="C9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="17" t="s">
         <v>15</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B10" s="13"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
+      <c r="C10" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>52</v>
+      </c>
       <c r="E10" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B11" s="13"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
+      <c r="C11" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>60</v>
+      </c>
       <c r="E11" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B12" s="13"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
+      <c r="C12" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>56</v>
+      </c>
       <c r="E12" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B13" s="13"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
+      <c r="C13" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>58</v>
+      </c>
       <c r="E13" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="14"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -990,9 +1008,13 @@
   <hyperlinks>
     <hyperlink ref="D9" r:id="rId1"/>
     <hyperlink ref="D8" r:id="rId2"/>
+    <hyperlink ref="D10" r:id="rId3"/>
+    <hyperlink ref="D12" r:id="rId4"/>
+    <hyperlink ref="D13" r:id="rId5"/>
+    <hyperlink ref="D11" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId7"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1005,29 +1027,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="1"/>
-    <col min="2" max="2" width="8.7109375" style="2"/>
-    <col min="3" max="3" width="8.7109375" style="1"/>
-    <col min="4" max="4" width="90.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="1" width="8.6640625" style="1"/>
+    <col min="2" max="2" width="8.6640625" style="2"/>
+    <col min="3" max="3" width="8.6640625" style="1"/>
+    <col min="4" max="4" width="90.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="31" t="s">
+    <row r="3" spans="2:5" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="33"/>
-    </row>
-    <row r="4" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="32"/>
+    </row>
+    <row r="4" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
         <v>0</v>
       </c>
@@ -1037,157 +1059,157 @@
       <c r="D4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="20" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C7" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="D15" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="1" t="s">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C18" s="20"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C18" s="19"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>

</xml_diff>